<commit_message>
imageupload,assetinfo,current asset info,asset register, asset schedule, data entry,frc system,header ,footer done
</commit_message>
<xml_diff>
--- a/afar_project/csv_path/excel_files/asset_register.xlsx
+++ b/afar_project/csv_path/excel_files/asset_register.xlsx
@@ -573,7 +573,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0001</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -682,7 +682,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0002</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -775,7 +775,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0003</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -868,7 +868,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0004</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0005</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1054,7 +1054,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0006</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0007</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0008</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0009</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-17-0010</t>
+          <t>FRC-HQ-SLM-C-17-0000</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-17-0011</t>
+          <t>FRC-HQ-SLM-C-17-0000</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0012</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1657,7 +1657,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0013</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0014</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0015</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0016</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2033,7 +2033,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0017</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2142,7 +2142,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0018</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2251,7 +2251,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0019</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2360,7 +2360,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0020</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2449,7 +2449,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0021</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2530,7 +2530,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0022</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2615,7 +2615,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0023</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2700,7 +2700,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0024</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2789,7 +2789,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0025</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0026</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2967,7 +2967,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0027</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3056,7 +3056,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0028</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3165,7 +3165,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0029</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3258,7 +3258,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0030</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3351,7 +3351,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0031</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3440,7 +3440,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0032</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3525,7 +3525,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0033</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3610,7 +3610,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0034</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3699,7 +3699,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0035</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3792,7 +3792,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0036</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3877,7 +3877,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0037</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3986,7 +3986,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0038</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4079,7 +4079,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0039</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4172,7 +4172,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0040</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -4265,7 +4265,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0041</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -4350,7 +4350,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0042</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4455,7 +4455,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0043</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4548,7 +4548,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0044</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -4637,7 +4637,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-17-0045</t>
+          <t>FRC-HQ-SLM-T-17-0000</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -4722,7 +4722,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-17-0046</t>
+          <t>FRC-HQ-SLM-T-17-0000</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -4803,7 +4803,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0047</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4912,7 +4912,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0048</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5021,7 +5021,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0049</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -5130,7 +5130,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0050</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -5235,7 +5235,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-17-0051</t>
+          <t>FRC-HQ-SLM-O-17-0000</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -5344,7 +5344,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0052</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -5449,7 +5449,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-17-0053</t>
+          <t>FRC-HQ-SLM-F-17-0000</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -5554,7 +5554,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0054</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -5659,7 +5659,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0055</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -5764,7 +5764,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0056</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -5873,7 +5873,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0057</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -5978,7 +5978,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0058</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -6083,7 +6083,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0059</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -6188,7 +6188,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0060</t>
+          <t>FRC-HQ-SLM-C-18-0000</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -6273,7 +6273,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0061</t>
+          <t>FRC-HQ-SLM-C-18-0000</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -6358,7 +6358,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0062</t>
+          <t>FRC-HQ-SLM-O-18-0000</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -6451,7 +6451,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0063</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -6540,7 +6540,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0064</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -6649,7 +6649,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0065</t>
+          <t>FRC-HQ-SLM-C-18-0000</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -6742,7 +6742,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0066</t>
+          <t>FRC-HQ-SLM-C-18-0000</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6827,7 +6827,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0067</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -6916,7 +6916,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0068</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -7005,7 +7005,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0069</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -7110,7 +7110,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0070</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -7199,7 +7199,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0071</t>
+          <t>FRC-HQ-SLM-C-18-0000</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -7284,7 +7284,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0072</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -7377,7 +7377,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0073</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -7466,7 +7466,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0074</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -7559,7 +7559,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0075</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -7652,7 +7652,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-18-0076</t>
+          <t>FRC-HQ-SLM-T-18-0000</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -7737,7 +7737,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0077</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -7830,7 +7830,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0078</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -7919,7 +7919,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0079</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -8004,7 +8004,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0080</t>
+          <t>FRC-HQ-SLM-C-18-0000</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -8097,7 +8097,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0081</t>
+          <t>FRC-HQ-SLM-C-18-0000</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -8186,7 +8186,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0082</t>
+          <t>FRC-HQ-SLM-C-18-0000</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -8279,7 +8279,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0083</t>
+          <t>FRC-HQ-SLM-C-18-0000</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -8372,7 +8372,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0084</t>
+          <t>FRC-HQ-SLM-O-18-0000</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -8457,7 +8457,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0085</t>
+          <t>FRC-HQ-SLM-C-18-0000</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -8550,7 +8550,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0086</t>
+          <t>FRC-HQ-SLM-C-18-0000</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -8643,7 +8643,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0087</t>
+          <t>FRC-HQ-SLM-O-18-0000</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -8728,7 +8728,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0088</t>
+          <t>FRC-HQ-SLM-C-18-0000</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -8813,7 +8813,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0089</t>
+          <t>FRC-HQ-SLM-C-18-0000</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -8906,7 +8906,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-18-0090</t>
+          <t>FRC-HQ-SLM-C-18-0000</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -8995,7 +8995,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0091</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -9100,7 +9100,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0092</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -9205,7 +9205,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0093</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -9310,7 +9310,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0094</t>
+          <t>FRC-HQ-SLM-O-18-0000</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -9419,7 +9419,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0095</t>
+          <t>FRC-HQ-SLM-F-18-0000</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -9504,7 +9504,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0096</t>
+          <t>FRC-HQ-SLM-O-18-0000</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -9589,7 +9589,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-18-0097</t>
+          <t>FRC-HQ-SLM-T-18-0000</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -9678,7 +9678,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-18-0098</t>
+          <t>FRC-HQ-SLM-M-18-0000</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -9771,7 +9771,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-18-0099</t>
+          <t>FRC-HQ-SLM-M-18-0000</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -9864,7 +9864,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0100</t>
+          <t>FRC-HQ-SLM-O-18-0001</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -9949,7 +9949,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0101</t>
+          <t>FRC-HQ-SLM-O-18-0001</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -10034,7 +10034,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0102</t>
+          <t>FRC-HQ-SLM-O-18-0001</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -10119,7 +10119,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0103</t>
+          <t>FRC-HQ-SLM-O-18-0001</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -10228,7 +10228,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0104</t>
+          <t>FRC-HQ-SLM-O-18-0001</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -10309,7 +10309,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0105</t>
+          <t>FRC-HQ-SLM-O-18-0001</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -10402,7 +10402,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0106</t>
+          <t>FRC-HQ-SLM-O-18-0001</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -10511,7 +10511,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0107</t>
+          <t>FRC-HQ-SLM-O-18-0001</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -10604,7 +10604,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0108</t>
+          <t>FRC-HQ-SLM-O-18-0001</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -10697,7 +10697,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-18-0109</t>
+          <t>FRC-HQ-SLM-O-18-0001</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -10782,7 +10782,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-18-0110</t>
+          <t>FRC-HQ-SLM-F-18-0001</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -10891,7 +10891,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0111</t>
+          <t>FRC-HQ-SLM-F-19-0001</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -10996,7 +10996,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0112</t>
+          <t>FRC-HQ-SLM-F-19-0001</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -11105,7 +11105,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0113</t>
+          <t>FRC-HQ-SLM-F-19-0001</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -11210,7 +11210,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0114</t>
+          <t>FRC-HQ-SLM-F-19-0001</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -11299,7 +11299,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0115</t>
+          <t>FRC-HQ-SLM-F-19-0001</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -11388,7 +11388,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0116</t>
+          <t>FRC-HQ-SLM-O-19-0001</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -11481,7 +11481,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0117</t>
+          <t>FRC-HQ-SLM-F-19-0001</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -11586,7 +11586,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0118</t>
+          <t>FRC-HQ-SLM-F-19-0001</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -11675,7 +11675,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0119</t>
+          <t>FRC-HQ-SLM-O-19-0001</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -11768,7 +11768,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0120</t>
+          <t>FRC-HQ-SLM-O-19-0001</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -11861,7 +11861,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0121</t>
+          <t>FRC-HQ-SLM-F-19-0001</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -11950,7 +11950,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-19-0122</t>
+          <t>FRC-HQ-SLM-C-19-0001</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -12043,7 +12043,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-19-0123</t>
+          <t>FRC-HQ-SLM-C-19-0001</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -12136,7 +12136,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-19-0124</t>
+          <t>FRC-HQ-SLM-C-19-0001</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -12229,7 +12229,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-19-0125</t>
+          <t>FRC-HQ-SLM-C-19-0001</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -12314,7 +12314,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0126</t>
+          <t>FRC-HQ-SLM-F-19-0001</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -12407,7 +12407,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0127</t>
+          <t>FRC-HQ-SLM-F-19-0001</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -12496,7 +12496,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-19-0128</t>
+          <t>FRC-HQ-SLM-F-19-0001</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -12585,7 +12585,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0129</t>
+          <t>FRC-HQ-SLM-C-20-0001</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -12674,7 +12674,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0130</t>
+          <t>FRC-HQ-SLM-C-20-0001</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -12767,7 +12767,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0131</t>
+          <t>FRC-HQ-SLM-C-20-0001</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -12860,7 +12860,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0132</t>
+          <t>FRC-HQ-SLM-C-20-0001</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -12949,7 +12949,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-20-0133</t>
+          <t>FRC-HQ-SLM-T-20-0001</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -13042,7 +13042,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0134</t>
+          <t>FRC-HQ-SLM-C-20-0001</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -13135,7 +13135,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0135</t>
+          <t>FRC-HQ-SLM-C-20-0001</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -13228,7 +13228,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0136</t>
+          <t>FRC-HQ-SLM-C-20-0001</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -13313,7 +13313,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0137</t>
+          <t>FRC-HQ-SLM-C-20-0001</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -13406,7 +13406,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-20-0138</t>
+          <t>FRC-HQ-SLM-F-20-0001</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -13499,7 +13499,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0139</t>
+          <t>FRC-HQ-SLM-C-20-0001</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -13592,7 +13592,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-20-0140</t>
+          <t>FRC-HQ-SLM-F-20-0001</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -13681,7 +13681,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0141</t>
+          <t>FRC-HQ-SLM-C-20-0001</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -13770,7 +13770,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-20-0142</t>
+          <t>FRC-HQ-SLM-C-20-0001</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -13863,7 +13863,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-21-0143</t>
+          <t>FRC-HQ-SLM-M-21-0001</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -13956,7 +13956,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-21-0144</t>
+          <t>FRC-HQ-SLM-M-21-0001</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -14037,7 +14037,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-21-0145</t>
+          <t>FRC-HQ-SLM-O-21-0001</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -14126,7 +14126,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0146</t>
+          <t>FRC-HQ-SLM-C-21-0001</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -14219,7 +14219,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0147</t>
+          <t>FRC-HQ-SLM-C-21-0001</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -14312,7 +14312,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-21-0148</t>
+          <t>FRC-HQ-SLM-M-21-0001</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -14393,7 +14393,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0149</t>
+          <t>FRC-HQ-SLM-F-21-0001</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -14486,7 +14486,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-21-0150</t>
+          <t>FRC-HQ-SLM-O-21-0001</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -14575,7 +14575,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0152</t>
+          <t>FRC-HQ-SLM-C-21-0001</t>
         </is>
       </c>
       <c r="F152" t="inlineStr"/>
@@ -14656,7 +14656,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0153</t>
+          <t>FRC-HQ-SLM-C-21-0001</t>
         </is>
       </c>
       <c r="F153" t="inlineStr"/>
@@ -14737,7 +14737,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0154</t>
+          <t>FRC-HQ-SLM-C-21-0001</t>
         </is>
       </c>
       <c r="F154" t="inlineStr"/>
@@ -14818,7 +14818,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0155</t>
+          <t>FRC-HQ-SLM-C-21-0001</t>
         </is>
       </c>
       <c r="F155" t="inlineStr"/>
@@ -14899,7 +14899,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0156</t>
+          <t>FRC-HQ-SLM-C-21-0001</t>
         </is>
       </c>
       <c r="F156" t="inlineStr"/>
@@ -14980,7 +14980,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0157</t>
+          <t>FRC-HQ-SLM-C-21-0001</t>
         </is>
       </c>
       <c r="F157" t="inlineStr"/>
@@ -15061,7 +15061,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0158</t>
+          <t>FRC-HQ-SLM-C-21-0001</t>
         </is>
       </c>
       <c r="F158" t="inlineStr"/>
@@ -15142,7 +15142,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0159</t>
+          <t>FRC-HQ-SLM-C-21-0001</t>
         </is>
       </c>
       <c r="F159" t="inlineStr"/>
@@ -15223,7 +15223,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0160</t>
+          <t>FRC-HQ-SLM-C-21-0001</t>
         </is>
       </c>
       <c r="F160" t="inlineStr"/>
@@ -15304,7 +15304,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-21-0161</t>
+          <t>FRC-HQ-SLM-C-21-0001</t>
         </is>
       </c>
       <c r="F161" t="inlineStr"/>
@@ -15385,7 +15385,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0162</t>
+          <t>FRC-HQ-SLM-I-21-0001</t>
         </is>
       </c>
       <c r="F162" t="inlineStr"/>
@@ -15466,7 +15466,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0163</t>
+          <t>FRC-HQ-SLM-I-21-0001</t>
         </is>
       </c>
       <c r="F163" t="inlineStr"/>
@@ -15547,7 +15547,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0164</t>
+          <t>FRC-HQ-SLM-I-21-0001</t>
         </is>
       </c>
       <c r="F164" t="inlineStr"/>
@@ -15628,7 +15628,7 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0165</t>
+          <t>FRC-HQ-SLM-I-21-0001</t>
         </is>
       </c>
       <c r="F165" t="inlineStr"/>
@@ -15709,7 +15709,7 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0166</t>
+          <t>FRC-HQ-SLM-I-21-0001</t>
         </is>
       </c>
       <c r="F166" t="inlineStr"/>
@@ -15790,7 +15790,7 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0167</t>
+          <t>FRC-HQ-SLM-I-21-0001</t>
         </is>
       </c>
       <c r="F167" t="inlineStr"/>
@@ -15871,7 +15871,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0168</t>
+          <t>FRC-HQ-SLM-I-21-0001</t>
         </is>
       </c>
       <c r="F168" t="inlineStr"/>
@@ -15952,7 +15952,7 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0169</t>
+          <t>FRC-HQ-SLM-I-21-0001</t>
         </is>
       </c>
       <c r="F169" t="inlineStr"/>
@@ -16034,7 +16034,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0170</t>
+          <t>FRC-HQ-SLM-I-21-0001</t>
         </is>
       </c>
       <c r="F170" t="inlineStr"/>
@@ -16119,7 +16119,7 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0171</t>
+          <t>FRC-HQ-SLM-I-21-0001</t>
         </is>
       </c>
       <c r="F171" t="inlineStr"/>
@@ -16200,7 +16200,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0172</t>
+          <t>FRC-HQ-SLM-I-21-0001</t>
         </is>
       </c>
       <c r="F172" t="inlineStr"/>
@@ -16285,7 +16285,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0173</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F173" t="inlineStr"/>
@@ -16370,7 +16370,7 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0174</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F174" t="inlineStr"/>
@@ -16455,7 +16455,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0175</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F175" t="inlineStr"/>
@@ -16540,7 +16540,7 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0176</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F176" t="inlineStr"/>
@@ -16621,7 +16621,7 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0177</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F177" t="inlineStr"/>
@@ -16702,7 +16702,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0178</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F178" t="inlineStr"/>
@@ -16783,7 +16783,7 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0179</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F179" t="inlineStr"/>
@@ -16864,7 +16864,7 @@
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0180</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F180" t="inlineStr"/>
@@ -16949,7 +16949,7 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0181</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F181" t="inlineStr"/>
@@ -17030,7 +17030,7 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0182</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F182" t="inlineStr"/>
@@ -17111,7 +17111,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0183</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F183" t="inlineStr"/>
@@ -17192,7 +17192,7 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0184</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F184" t="inlineStr"/>
@@ -17274,7 +17274,7 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0185</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F185" t="inlineStr"/>
@@ -17355,7 +17355,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0186</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F186" t="inlineStr"/>
@@ -17436,7 +17436,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0187</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F187" t="inlineStr"/>
@@ -17517,7 +17517,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0188</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F188" t="inlineStr"/>
@@ -17598,7 +17598,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0189</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F189" t="inlineStr"/>
@@ -17679,7 +17679,7 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0190</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F190" t="inlineStr"/>
@@ -17764,7 +17764,7 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0191</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F191" t="inlineStr"/>
@@ -17849,7 +17849,7 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0192</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F192" t="inlineStr"/>
@@ -17930,7 +17930,7 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0193</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F193" t="inlineStr"/>
@@ -18015,7 +18015,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0194</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F194" t="inlineStr"/>
@@ -18100,7 +18100,7 @@
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0195</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F195" t="inlineStr"/>
@@ -18185,7 +18185,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0196</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F196" t="inlineStr"/>
@@ -18266,7 +18266,7 @@
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-S-21-0197</t>
+          <t>FRC-HQ-SLM-S-21-0001</t>
         </is>
       </c>
       <c r="F197" t="inlineStr"/>
@@ -18347,7 +18347,7 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0198</t>
+          <t>FRC-HQ-SLM-E-21-0001</t>
         </is>
       </c>
       <c r="F198" t="inlineStr"/>
@@ -18432,7 +18432,7 @@
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0199</t>
+          <t>FRC-HQ-SLM-E-21-0001</t>
         </is>
       </c>
       <c r="F199" t="inlineStr"/>
@@ -18517,7 +18517,7 @@
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0200</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F200" t="inlineStr"/>
@@ -18602,7 +18602,7 @@
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0201</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F201" t="inlineStr"/>
@@ -18687,7 +18687,7 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0202</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F202" t="inlineStr"/>
@@ -18772,7 +18772,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0203</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F203" t="inlineStr"/>
@@ -18857,7 +18857,7 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0204</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F204" t="inlineStr"/>
@@ -18942,7 +18942,7 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0205</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F205" t="inlineStr"/>
@@ -19027,7 +19027,7 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0206</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F206" t="inlineStr"/>
@@ -19112,7 +19112,7 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0207</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F207" t="inlineStr"/>
@@ -19197,7 +19197,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0208</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F208" t="inlineStr"/>
@@ -19282,7 +19282,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0209</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F209" t="inlineStr"/>
@@ -19367,7 +19367,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0210</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F210" t="inlineStr"/>
@@ -19452,7 +19452,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0211</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F211" t="inlineStr"/>
@@ -19537,7 +19537,7 @@
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0212</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F212" t="inlineStr"/>
@@ -19622,7 +19622,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0213</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F213" t="inlineStr"/>
@@ -19707,7 +19707,7 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0214</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F214" t="inlineStr"/>
@@ -19792,7 +19792,7 @@
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0215</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F215" t="inlineStr"/>
@@ -19877,7 +19877,7 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0216</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F216" t="inlineStr"/>
@@ -19962,7 +19962,7 @@
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0217</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F217" t="inlineStr"/>
@@ -20047,7 +20047,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0218</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F218" t="inlineStr"/>
@@ -20136,7 +20136,7 @@
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0219</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F219" t="inlineStr"/>
@@ -20225,7 +20225,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0220</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F220" t="inlineStr"/>
@@ -20310,7 +20310,7 @@
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0221</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F221" t="inlineStr"/>
@@ -20395,7 +20395,7 @@
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0222</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F222" t="inlineStr"/>
@@ -20476,7 +20476,7 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0223</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F223" t="inlineStr"/>
@@ -20557,7 +20557,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0224</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F224" t="inlineStr"/>
@@ -20642,7 +20642,7 @@
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0225</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F225" t="inlineStr"/>
@@ -20727,7 +20727,7 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0226</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F226" t="inlineStr"/>
@@ -20812,7 +20812,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0227</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F227" t="inlineStr"/>
@@ -20897,7 +20897,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0228</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F228" t="inlineStr"/>
@@ -20978,7 +20978,7 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0229</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F229" t="inlineStr"/>
@@ -21059,7 +21059,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0230</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F230" t="inlineStr"/>
@@ -21140,7 +21140,7 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0231</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F231" t="inlineStr"/>
@@ -21221,7 +21221,7 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0232</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F232" t="inlineStr"/>
@@ -21302,7 +21302,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0233</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F233" t="inlineStr"/>
@@ -21383,7 +21383,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0234</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F234" t="inlineStr"/>
@@ -21464,7 +21464,7 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0235</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F235" t="inlineStr"/>
@@ -21549,7 +21549,7 @@
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-21-0236</t>
+          <t>FRC-HQ-SLM-E-21-0002</t>
         </is>
       </c>
       <c r="F236" t="inlineStr"/>
@@ -21634,7 +21634,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-21-0237</t>
+          <t>FRC-HQ-SLM-P-21-0002</t>
         </is>
       </c>
       <c r="F237" t="inlineStr"/>
@@ -21715,7 +21715,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-21-0238</t>
+          <t>FRC-HQ-SLM-P-21-0002</t>
         </is>
       </c>
       <c r="F238" t="inlineStr"/>
@@ -21796,7 +21796,7 @@
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-21-0239</t>
+          <t>FRC-HQ-SLM-P-21-0002</t>
         </is>
       </c>
       <c r="F239" t="inlineStr"/>
@@ -21877,7 +21877,7 @@
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-21-0240</t>
+          <t>FRC-HQ-SLM-P-21-0002</t>
         </is>
       </c>
       <c r="F240" t="inlineStr"/>
@@ -21958,7 +21958,7 @@
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-P-21-0241</t>
+          <t>FRC-HQ-SLM-P-21-0002</t>
         </is>
       </c>
       <c r="F241" t="inlineStr"/>
@@ -22039,7 +22039,7 @@
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0242</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F242" t="inlineStr"/>
@@ -22120,7 +22120,7 @@
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0243</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F243" t="inlineStr"/>
@@ -22201,7 +22201,7 @@
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0244</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F244" t="inlineStr"/>
@@ -22282,7 +22282,7 @@
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0245</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F245" t="inlineStr"/>
@@ -22363,7 +22363,7 @@
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0246</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F246" t="inlineStr"/>
@@ -22444,7 +22444,7 @@
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0247</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F247" t="inlineStr"/>
@@ -22525,7 +22525,7 @@
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0248</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F248" t="inlineStr"/>
@@ -22606,7 +22606,7 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0249</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F249" t="inlineStr"/>
@@ -22687,7 +22687,7 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0250</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F250" t="inlineStr"/>
@@ -22768,7 +22768,7 @@
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0251</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F251" t="inlineStr"/>
@@ -22849,7 +22849,7 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0252</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F252" t="inlineStr"/>
@@ -22930,7 +22930,7 @@
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0253</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F253" t="inlineStr"/>
@@ -23011,7 +23011,7 @@
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0254</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F254" t="inlineStr"/>
@@ -23092,7 +23092,7 @@
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0255</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F255" t="inlineStr"/>
@@ -23173,7 +23173,7 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0256</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F256" t="inlineStr"/>
@@ -23254,7 +23254,7 @@
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0257</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F257" t="inlineStr"/>
@@ -23335,7 +23335,7 @@
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0258</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F258" t="inlineStr"/>
@@ -23416,7 +23416,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0259</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F259" t="inlineStr"/>
@@ -23497,7 +23497,7 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0260</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F260" t="inlineStr"/>
@@ -23578,7 +23578,7 @@
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0261</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F261" t="inlineStr"/>
@@ -23659,7 +23659,7 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0262</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F262" t="inlineStr"/>
@@ -23740,7 +23740,7 @@
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0263</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F263" t="inlineStr"/>
@@ -23821,7 +23821,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0264</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F264" t="inlineStr"/>
@@ -23902,7 +23902,7 @@
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0265</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F265" t="inlineStr"/>
@@ -23983,7 +23983,7 @@
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0266</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F266" t="inlineStr"/>
@@ -24064,7 +24064,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0267</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F267" t="inlineStr"/>
@@ -24145,7 +24145,7 @@
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0268</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F268" t="inlineStr"/>
@@ -24226,7 +24226,7 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0269</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F269" t="inlineStr"/>
@@ -24311,7 +24311,7 @@
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0270</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F270" t="inlineStr"/>
@@ -24392,7 +24392,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0271</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F271" t="inlineStr"/>
@@ -24473,7 +24473,7 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0272</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F272" t="inlineStr"/>
@@ -24554,7 +24554,7 @@
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0273</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F273" t="inlineStr"/>
@@ -24635,7 +24635,7 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-I-21-0274</t>
+          <t>FRC-HQ-SLM-I-21-0002</t>
         </is>
       </c>
       <c r="F274" t="inlineStr"/>
@@ -24716,7 +24716,7 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0275</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F275" t="inlineStr"/>
@@ -24797,7 +24797,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0276</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F276" t="inlineStr"/>
@@ -24878,7 +24878,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0277</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F277" t="inlineStr"/>
@@ -24959,7 +24959,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0278</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F278" t="inlineStr"/>
@@ -25040,7 +25040,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0279</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F279" t="inlineStr"/>
@@ -25121,7 +25121,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0280</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F280" t="inlineStr"/>
@@ -25202,7 +25202,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0281</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F281" t="inlineStr"/>
@@ -25283,7 +25283,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0282</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F282" t="inlineStr"/>
@@ -25364,7 +25364,7 @@
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0283</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F283" t="inlineStr"/>
@@ -25445,7 +25445,7 @@
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0284</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F284" t="inlineStr"/>
@@ -25530,7 +25530,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0285</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F285" t="inlineStr"/>
@@ -25615,7 +25615,7 @@
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0286</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F286" t="inlineStr"/>
@@ -25700,7 +25700,7 @@
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0287</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F287" t="inlineStr"/>
@@ -25781,7 +25781,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0288</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F288" t="inlineStr"/>
@@ -25866,7 +25866,7 @@
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0289</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F289" t="inlineStr"/>
@@ -25951,7 +25951,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0290</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F290" t="inlineStr"/>
@@ -26036,7 +26036,7 @@
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0291</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F291" t="inlineStr"/>
@@ -26121,7 +26121,7 @@
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0292</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F292" t="inlineStr"/>
@@ -26206,7 +26206,7 @@
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0293</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F293" t="inlineStr"/>
@@ -26291,7 +26291,7 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0294</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F294" t="inlineStr"/>
@@ -26376,7 +26376,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0295</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F295" t="inlineStr"/>
@@ -26461,7 +26461,7 @@
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0296</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F296" t="inlineStr"/>
@@ -26542,7 +26542,7 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0297</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F297" t="inlineStr"/>
@@ -26623,7 +26623,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0298</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F298" t="inlineStr"/>
@@ -26704,7 +26704,7 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0299</t>
+          <t>FRC-HQ-SLM-F-21-0002</t>
         </is>
       </c>
       <c r="F299" t="inlineStr"/>
@@ -26785,7 +26785,7 @@
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0300</t>
+          <t>FRC-HQ-SLM-F-21-0003</t>
         </is>
       </c>
       <c r="F300" t="inlineStr"/>
@@ -26866,7 +26866,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0301</t>
+          <t>FRC-HQ-SLM-F-21-0003</t>
         </is>
       </c>
       <c r="F301" t="inlineStr"/>
@@ -26947,7 +26947,7 @@
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-23-0001</t>
+          <t>FRC-HQ-SLM-F-23-0000</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -27028,7 +27028,7 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-23-0001</t>
+          <t>FRC-HQ-SLM-F-23-0000</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
@@ -27109,7 +27109,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-23-0002</t>
+          <t>FRC-HQ-SLM-M-23-0000</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -27190,7 +27190,7 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-23-0002</t>
+          <t>FRC-HQ-SLM-M-23-0000</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -27271,7 +27271,7 @@
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-23-0002</t>
+          <t>FRC-HQ-SLM-M-23-0000</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -27352,7 +27352,7 @@
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-M-23-0002</t>
+          <t>FRC-HQ-SLM-M-23-0000</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -27433,7 +27433,7 @@
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0003</t>
+          <t>FRC-HQ-SLM-F-21-0000</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -27514,7 +27514,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-21-0003</t>
+          <t>FRC-HQ-SLM-F-21-0000</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -27595,7 +27595,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0006</t>
+          <t>FRC-HQ-SLM-O-19-0000</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -27676,7 +27676,7 @@
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-19-0006</t>
+          <t>FRC-HQ-SLM-O-19-0000</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
@@ -27757,7 +27757,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-23-0006</t>
+          <t>FRC-HQ-SLM-F-23-0000</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -27838,7 +27838,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-F-23-0006</t>
+          <t>FRC-HQ-SLM-F-23-0000</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -27919,7 +27919,7 @@
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-23-0006</t>
+          <t>FRC-HQ-SLM-T-23-0000</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -28000,7 +28000,7 @@
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-23-0006</t>
+          <t>FRC-HQ-SLM-T-23-0000</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
@@ -28081,7 +28081,7 @@
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-23-0006</t>
+          <t>FRC-HQ-SLM-E-23-0000</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -28162,7 +28162,7 @@
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-23-0006</t>
+          <t>FRC-HQ-SLM-E-23-0000</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
@@ -28243,7 +28243,7 @@
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-E-23-0006</t>
+          <t>FRC-HQ-SLM-E-23-0000</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
@@ -28324,7 +28324,7 @@
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0006</t>
+          <t>FRC-HQ-SLM-C-22-0000</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
@@ -28405,7 +28405,7 @@
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-22-0006</t>
+          <t>FRC-HQ-SLM-C-22-0000</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
@@ -28486,7 +28486,7 @@
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-HQ-SLM-C-23-0000</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
@@ -28567,7 +28567,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-HQ-SLM-C-23-0000</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
@@ -28648,7 +28648,7 @@
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-HQ-SLM-C-23-0000</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
@@ -28729,7 +28729,7 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-HQ-SLM-C-23-0000</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -28810,7 +28810,7 @@
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-HQ-SLM-C-23-0000</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
@@ -28891,7 +28891,7 @@
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-HQ-SLM-C-23-0000</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
@@ -28972,7 +28972,7 @@
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-HQ-SLM-C-23-0000</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
@@ -29053,7 +29053,7 @@
       </c>
       <c r="E328" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-HQ-SLM-C-23-0000</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">
@@ -29134,7 +29134,7 @@
       </c>
       <c r="E329" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-HQ-SLM-C-23-0000</t>
         </is>
       </c>
       <c r="F329" t="inlineStr">
@@ -29215,7 +29215,7 @@
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-HQ-SLM-C-23-0000</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
@@ -29296,7 +29296,7 @@
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-HQ-SLM-C-23-0000</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
@@ -29377,7 +29377,7 @@
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-C-23-0001</t>
+          <t>FRC-HQ-SLM-C-23-0000</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
@@ -29458,7 +29458,7 @@
       </c>
       <c r="E333" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-T-20-0001</t>
+          <t>FRC-HQ-SLM-T-20-0000</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
@@ -29539,7 +29539,7 @@
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t>FRC-HQ-SLM-O-21-0001</t>
+          <t>FRC-HQ-SLM-O-21-0000</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">

</xml_diff>